<commit_message>
fix contador materias completadas
</commit_message>
<xml_diff>
--- a/adultos2000.xlsx
+++ b/adultos2000.xlsx
@@ -261,49 +261,7 @@
     <cellStyle name="Encabezado 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -632,7 +590,7 @@
   <dimension ref="B1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,8 +711,12 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="6">
+        <v>42637</v>
+      </c>
+      <c r="D6" s="5">
+        <v>9</v>
+      </c>
       <c r="E6" s="5" t="s">
         <v>13</v>
       </c>
@@ -884,7 +846,7 @@
       </c>
       <c r="C17" s="2">
         <f>+AVERAGE(D2:D14,G2:G14,J2:J14)</f>
-        <v>8</v>
+        <v>8.3333333333333339</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -901,8 +863,8 @@
         <v>30</v>
       </c>
       <c r="C19" s="2">
-        <f>+COUNTA(D2:D14)</f>
-        <v>2</v>
+        <f>+COUNTA(D2:D14,G2:G14,J2:J14)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -911,7 +873,7 @@
       </c>
       <c r="C20" s="2">
         <f>+C18-C19</f>
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>